<commit_message>
update: adicionar mais de um valor & validação dos valores
</commit_message>
<xml_diff>
--- a/planilhas/2024/Maio 2024.xlsx
+++ b/planilhas/2024/Maio 2024.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Soma" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Dia 20" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Dia 21" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Dia 25" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -522,7 +523,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="9.43357142857143" bestFit="1" customWidth="1" style="15" min="1" max="1"/>
     <col width="11.14785714285714" bestFit="1" customWidth="1" style="16" min="2" max="2"/>
@@ -1673,24 +1674,24 @@
         </is>
       </c>
       <c r="B26" s="11" t="n">
-        <v>0</v>
+        <v>2060</v>
       </c>
       <c r="C26" s="11" t="n">
-        <v>0</v>
+        <v>1030</v>
       </c>
       <c r="D26" s="11" t="n">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="E26" s="8" t="n"/>
       <c r="F26" s="11" t="n">
-        <v>0</v>
+        <v>3370</v>
       </c>
       <c r="G26" s="8" t="n"/>
       <c r="H26" s="12" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="11" t="n">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="J26" s="8" t="n"/>
       <c r="K26" s="13" t="n"/>
@@ -1988,7 +1989,7 @@
         </is>
       </c>
       <c r="I33" s="14" t="n">
-        <v>24760</v>
+        <v>25110</v>
       </c>
       <c r="J33" s="8" t="n"/>
       <c r="K33" s="13" t="n"/>
@@ -2781,7 +2782,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
@@ -2881,4 +2882,147 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Débito</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Crédito</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Parcelas</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>100</v>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>130</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>120</v>
+      </c>
+      <c r="B3" t="n">
+        <v>130</v>
+      </c>
+      <c r="C3" t="n">
+        <v>150</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>130</v>
+      </c>
+      <c r="B4" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>120</v>
+      </c>
+      <c r="B5" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>120</v>
+      </c>
+      <c r="B6" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>130</v>
+      </c>
+      <c r="B7" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>150</v>
+      </c>
+      <c r="B8" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>